<commit_message>
Update on 20250622 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/IPV6直播源汇总/海南移动.xlsx
+++ b/直播源汇总文档/IPV6直播源汇总/海南移动.xlsx
@@ -14026,7 +14026,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>410</v>
+        <v>4</v>
       </c>
       <c r="B62" t="s">
         <v>439</v>
@@ -14038,7 +14038,7 @@
         <v>441</v>
       </c>
       <c r="E62" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F62" t="s">
         <v>454</v>
@@ -14046,7 +14046,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>410</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
         <v>439</v>
@@ -14058,7 +14058,7 @@
         <v>451</v>
       </c>
       <c r="E63" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F63" t="s">
         <v>454</v>
@@ -14066,7 +14066,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>410</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
         <v>439</v>
@@ -14078,7 +14078,7 @@
         <v>449</v>
       </c>
       <c r="E64" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F64" t="s">
         <v>454</v>
@@ -14086,7 +14086,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>410</v>
+        <v>4</v>
       </c>
       <c r="B65" t="s">
         <v>439</v>
@@ -14098,7 +14098,7 @@
         <v>445</v>
       </c>
       <c r="E65" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F65" t="s">
         <v>454</v>
@@ -14106,7 +14106,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>410</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
         <v>439</v>
@@ -14118,7 +14118,7 @@
         <v>443</v>
       </c>
       <c r="E66" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F66" t="s">
         <v>454</v>
@@ -14126,7 +14126,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>410</v>
+        <v>4</v>
       </c>
       <c r="B67" t="s">
         <v>439</v>
@@ -14138,7 +14138,7 @@
         <v>447</v>
       </c>
       <c r="E67" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F67" t="s">
         <v>454</v>
@@ -14158,7 +14158,7 @@
         <v>441</v>
       </c>
       <c r="E68" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="F68" t="s">
         <v>454</v>
@@ -14178,7 +14178,7 @@
         <v>451</v>
       </c>
       <c r="E69" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="F69" t="s">
         <v>454</v>
@@ -14198,7 +14198,7 @@
         <v>449</v>
       </c>
       <c r="E70" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="F70" t="s">
         <v>454</v>
@@ -14218,7 +14218,7 @@
         <v>445</v>
       </c>
       <c r="E71" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="F71" t="s">
         <v>454</v>
@@ -14238,7 +14238,7 @@
         <v>443</v>
       </c>
       <c r="E72" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="F72" t="s">
         <v>454</v>
@@ -14258,7 +14258,7 @@
         <v>447</v>
       </c>
       <c r="E73" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="F73" t="s">
         <v>454</v>
@@ -14278,7 +14278,7 @@
         <v>441</v>
       </c>
       <c r="E74" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="F74" t="s">
         <v>454</v>
@@ -14298,7 +14298,7 @@
         <v>451</v>
       </c>
       <c r="E75" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="F75" t="s">
         <v>454</v>
@@ -14318,7 +14318,7 @@
         <v>449</v>
       </c>
       <c r="E76" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="F76" t="s">
         <v>454</v>
@@ -14338,7 +14338,7 @@
         <v>445</v>
       </c>
       <c r="E77" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="F77" t="s">
         <v>454</v>
@@ -14358,7 +14358,7 @@
         <v>443</v>
       </c>
       <c r="E78" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="F78" t="s">
         <v>454</v>
@@ -14378,7 +14378,7 @@
         <v>447</v>
       </c>
       <c r="E79" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="F79" t="s">
         <v>454</v>
@@ -14398,7 +14398,7 @@
         <v>441</v>
       </c>
       <c r="E80" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F80" t="s">
         <v>454</v>
@@ -14418,7 +14418,7 @@
         <v>451</v>
       </c>
       <c r="E81" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F81" t="s">
         <v>454</v>
@@ -14438,7 +14438,7 @@
         <v>449</v>
       </c>
       <c r="E82" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F82" t="s">
         <v>454</v>
@@ -14458,7 +14458,7 @@
         <v>445</v>
       </c>
       <c r="E83" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F83" t="s">
         <v>454</v>
@@ -14478,7 +14478,7 @@
         <v>443</v>
       </c>
       <c r="E84" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F84" t="s">
         <v>454</v>
@@ -14498,7 +14498,7 @@
         <v>447</v>
       </c>
       <c r="E85" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F85" t="s">
         <v>454</v>
@@ -14518,7 +14518,7 @@
         <v>441</v>
       </c>
       <c r="E86" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F86" t="s">
         <v>454</v>
@@ -14538,7 +14538,7 @@
         <v>451</v>
       </c>
       <c r="E87" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F87" t="s">
         <v>454</v>
@@ -14558,7 +14558,7 @@
         <v>449</v>
       </c>
       <c r="E88" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F88" t="s">
         <v>454</v>
@@ -14578,7 +14578,7 @@
         <v>445</v>
       </c>
       <c r="E89" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F89" t="s">
         <v>454</v>
@@ -14598,7 +14598,7 @@
         <v>443</v>
       </c>
       <c r="E90" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F90" t="s">
         <v>454</v>
@@ -14618,7 +14618,7 @@
         <v>447</v>
       </c>
       <c r="E91" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F91" t="s">
         <v>454</v>
@@ -14626,7 +14626,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="B92" t="s">
         <v>439</v>
@@ -14638,7 +14638,7 @@
         <v>441</v>
       </c>
       <c r="E92" t="s">
-        <v>312</v>
+        <v>210</v>
       </c>
       <c r="F92" t="s">
         <v>454</v>
@@ -14646,7 +14646,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="B93" t="s">
         <v>439</v>
@@ -14658,7 +14658,7 @@
         <v>451</v>
       </c>
       <c r="E93" t="s">
-        <v>312</v>
+        <v>210</v>
       </c>
       <c r="F93" t="s">
         <v>454</v>
@@ -14666,7 +14666,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="B94" t="s">
         <v>439</v>
@@ -14678,7 +14678,7 @@
         <v>449</v>
       </c>
       <c r="E94" t="s">
-        <v>312</v>
+        <v>210</v>
       </c>
       <c r="F94" t="s">
         <v>454</v>
@@ -14686,7 +14686,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="B95" t="s">
         <v>439</v>
@@ -14698,7 +14698,7 @@
         <v>445</v>
       </c>
       <c r="E95" t="s">
-        <v>312</v>
+        <v>210</v>
       </c>
       <c r="F95" t="s">
         <v>454</v>
@@ -14706,7 +14706,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="B96" t="s">
         <v>439</v>
@@ -14718,7 +14718,7 @@
         <v>443</v>
       </c>
       <c r="E96" t="s">
-        <v>312</v>
+        <v>210</v>
       </c>
       <c r="F96" t="s">
         <v>454</v>
@@ -14726,7 +14726,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="B97" t="s">
         <v>439</v>
@@ -14738,7 +14738,7 @@
         <v>447</v>
       </c>
       <c r="E97" t="s">
-        <v>312</v>
+        <v>210</v>
       </c>
       <c r="F97" t="s">
         <v>454</v>
@@ -21106,7 +21106,7 @@
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A416" t="s">
-        <v>1</v>
+        <v>442</v>
       </c>
       <c r="B416" t="s">
         <v>439</v>
@@ -21118,7 +21118,7 @@
         <v>441</v>
       </c>
       <c r="E416" t="s">
-        <v>30</v>
+        <v>363</v>
       </c>
       <c r="F416" t="s">
         <v>454</v>
@@ -21126,7 +21126,7 @@
     </row>
     <row r="417" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A417" t="s">
-        <v>1</v>
+        <v>442</v>
       </c>
       <c r="B417" t="s">
         <v>439</v>
@@ -21138,7 +21138,7 @@
         <v>451</v>
       </c>
       <c r="E417" t="s">
-        <v>30</v>
+        <v>363</v>
       </c>
       <c r="F417" t="s">
         <v>454</v>
@@ -21146,7 +21146,7 @@
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A418" t="s">
-        <v>1</v>
+        <v>442</v>
       </c>
       <c r="B418" t="s">
         <v>439</v>
@@ -21158,7 +21158,7 @@
         <v>449</v>
       </c>
       <c r="E418" t="s">
-        <v>30</v>
+        <v>363</v>
       </c>
       <c r="F418" t="s">
         <v>454</v>
@@ -21166,7 +21166,7 @@
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A419" t="s">
-        <v>1</v>
+        <v>442</v>
       </c>
       <c r="B419" t="s">
         <v>439</v>
@@ -21178,7 +21178,7 @@
         <v>445</v>
       </c>
       <c r="E419" t="s">
-        <v>30</v>
+        <v>363</v>
       </c>
       <c r="F419" t="s">
         <v>454</v>
@@ -21186,7 +21186,7 @@
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A420" t="s">
-        <v>1</v>
+        <v>442</v>
       </c>
       <c r="B420" t="s">
         <v>439</v>
@@ -21198,7 +21198,7 @@
         <v>443</v>
       </c>
       <c r="E420" t="s">
-        <v>30</v>
+        <v>363</v>
       </c>
       <c r="F420" t="s">
         <v>454</v>
@@ -21206,7 +21206,7 @@
     </row>
     <row r="421" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A421" t="s">
-        <v>1</v>
+        <v>442</v>
       </c>
       <c r="B421" t="s">
         <v>439</v>
@@ -21218,7 +21218,7 @@
         <v>447</v>
       </c>
       <c r="E421" t="s">
-        <v>30</v>
+        <v>363</v>
       </c>
       <c r="F421" t="s">
         <v>454</v>
@@ -21238,7 +21238,7 @@
         <v>441</v>
       </c>
       <c r="E422" t="s">
-        <v>258</v>
+        <v>30</v>
       </c>
       <c r="F422" t="s">
         <v>454</v>
@@ -21258,7 +21258,7 @@
         <v>451</v>
       </c>
       <c r="E423" t="s">
-        <v>258</v>
+        <v>30</v>
       </c>
       <c r="F423" t="s">
         <v>454</v>
@@ -21278,7 +21278,7 @@
         <v>449</v>
       </c>
       <c r="E424" t="s">
-        <v>258</v>
+        <v>30</v>
       </c>
       <c r="F424" t="s">
         <v>454</v>
@@ -21298,7 +21298,7 @@
         <v>445</v>
       </c>
       <c r="E425" t="s">
-        <v>258</v>
+        <v>30</v>
       </c>
       <c r="F425" t="s">
         <v>454</v>
@@ -21318,7 +21318,7 @@
         <v>443</v>
       </c>
       <c r="E426" t="s">
-        <v>258</v>
+        <v>30</v>
       </c>
       <c r="F426" t="s">
         <v>454</v>
@@ -21338,7 +21338,7 @@
         <v>447</v>
       </c>
       <c r="E427" t="s">
-        <v>258</v>
+        <v>30</v>
       </c>
       <c r="F427" t="s">
         <v>454</v>
@@ -21358,7 +21358,7 @@
         <v>441</v>
       </c>
       <c r="E428" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
       <c r="F428" t="s">
         <v>454</v>
@@ -21378,7 +21378,7 @@
         <v>451</v>
       </c>
       <c r="E429" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
       <c r="F429" t="s">
         <v>454</v>
@@ -21398,7 +21398,7 @@
         <v>449</v>
       </c>
       <c r="E430" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
       <c r="F430" t="s">
         <v>454</v>
@@ -21418,7 +21418,7 @@
         <v>445</v>
       </c>
       <c r="E431" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
       <c r="F431" t="s">
         <v>454</v>
@@ -21438,7 +21438,7 @@
         <v>443</v>
       </c>
       <c r="E432" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
       <c r="F432" t="s">
         <v>454</v>
@@ -21458,7 +21458,7 @@
         <v>447</v>
       </c>
       <c r="E433" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
       <c r="F433" t="s">
         <v>454</v>
@@ -21478,7 +21478,7 @@
         <v>441</v>
       </c>
       <c r="E434" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F434" t="s">
         <v>454</v>
@@ -21498,7 +21498,7 @@
         <v>451</v>
       </c>
       <c r="E435" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F435" t="s">
         <v>454</v>
@@ -21518,7 +21518,7 @@
         <v>449</v>
       </c>
       <c r="E436" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F436" t="s">
         <v>454</v>
@@ -21538,7 +21538,7 @@
         <v>445</v>
       </c>
       <c r="E437" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F437" t="s">
         <v>454</v>
@@ -21558,7 +21558,7 @@
         <v>443</v>
       </c>
       <c r="E438" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F438" t="s">
         <v>454</v>
@@ -21578,7 +21578,7 @@
         <v>447</v>
       </c>
       <c r="E439" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F439" t="s">
         <v>454</v>
@@ -21586,7 +21586,7 @@
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A440" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="B440" t="s">
         <v>439</v>
@@ -21598,7 +21598,7 @@
         <v>441</v>
       </c>
       <c r="E440" t="s">
-        <v>206</v>
+        <v>323</v>
       </c>
       <c r="F440" t="s">
         <v>454</v>
@@ -21606,7 +21606,7 @@
     </row>
     <row r="441" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A441" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="B441" t="s">
         <v>439</v>
@@ -21618,7 +21618,7 @@
         <v>451</v>
       </c>
       <c r="E441" t="s">
-        <v>206</v>
+        <v>323</v>
       </c>
       <c r="F441" t="s">
         <v>454</v>
@@ -21626,7 +21626,7 @@
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A442" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="B442" t="s">
         <v>439</v>
@@ -21638,7 +21638,7 @@
         <v>449</v>
       </c>
       <c r="E442" t="s">
-        <v>206</v>
+        <v>323</v>
       </c>
       <c r="F442" t="s">
         <v>454</v>
@@ -21646,7 +21646,7 @@
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A443" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="B443" t="s">
         <v>439</v>
@@ -21658,7 +21658,7 @@
         <v>445</v>
       </c>
       <c r="E443" t="s">
-        <v>206</v>
+        <v>323</v>
       </c>
       <c r="F443" t="s">
         <v>454</v>
@@ -21666,7 +21666,7 @@
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A444" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="B444" t="s">
         <v>439</v>
@@ -21678,7 +21678,7 @@
         <v>443</v>
       </c>
       <c r="E444" t="s">
-        <v>206</v>
+        <v>323</v>
       </c>
       <c r="F444" t="s">
         <v>454</v>
@@ -21686,7 +21686,7 @@
     </row>
     <row r="445" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A445" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="B445" t="s">
         <v>439</v>
@@ -21698,7 +21698,7 @@
         <v>447</v>
       </c>
       <c r="E445" t="s">
-        <v>206</v>
+        <v>323</v>
       </c>
       <c r="F445" t="s">
         <v>454</v>
@@ -21718,7 +21718,7 @@
         <v>441</v>
       </c>
       <c r="E446" t="s">
-        <v>339</v>
+        <v>206</v>
       </c>
       <c r="F446" t="s">
         <v>454</v>
@@ -21738,7 +21738,7 @@
         <v>451</v>
       </c>
       <c r="E447" t="s">
-        <v>339</v>
+        <v>206</v>
       </c>
       <c r="F447" t="s">
         <v>454</v>
@@ -21758,7 +21758,7 @@
         <v>449</v>
       </c>
       <c r="E448" t="s">
-        <v>339</v>
+        <v>206</v>
       </c>
       <c r="F448" t="s">
         <v>454</v>
@@ -21778,7 +21778,7 @@
         <v>445</v>
       </c>
       <c r="E449" t="s">
-        <v>339</v>
+        <v>206</v>
       </c>
       <c r="F449" t="s">
         <v>454</v>
@@ -21798,7 +21798,7 @@
         <v>443</v>
       </c>
       <c r="E450" t="s">
-        <v>339</v>
+        <v>206</v>
       </c>
       <c r="F450" t="s">
         <v>454</v>
@@ -21818,7 +21818,7 @@
         <v>447</v>
       </c>
       <c r="E451" t="s">
-        <v>339</v>
+        <v>206</v>
       </c>
       <c r="F451" t="s">
         <v>454</v>
@@ -21826,7 +21826,7 @@
     </row>
     <row r="452" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A452" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B452" t="s">
         <v>439</v>
@@ -21838,7 +21838,7 @@
         <v>441</v>
       </c>
       <c r="E452" t="s">
-        <v>208</v>
+        <v>339</v>
       </c>
       <c r="F452" t="s">
         <v>454</v>
@@ -21846,7 +21846,7 @@
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A453" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B453" t="s">
         <v>439</v>
@@ -21858,7 +21858,7 @@
         <v>451</v>
       </c>
       <c r="E453" t="s">
-        <v>208</v>
+        <v>339</v>
       </c>
       <c r="F453" t="s">
         <v>454</v>
@@ -21866,7 +21866,7 @@
     </row>
     <row r="454" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A454" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B454" t="s">
         <v>439</v>
@@ -21878,7 +21878,7 @@
         <v>449</v>
       </c>
       <c r="E454" t="s">
-        <v>208</v>
+        <v>339</v>
       </c>
       <c r="F454" t="s">
         <v>454</v>
@@ -21886,7 +21886,7 @@
     </row>
     <row r="455" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A455" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B455" t="s">
         <v>439</v>
@@ -21898,7 +21898,7 @@
         <v>445</v>
       </c>
       <c r="E455" t="s">
-        <v>208</v>
+        <v>339</v>
       </c>
       <c r="F455" t="s">
         <v>454</v>
@@ -21906,7 +21906,7 @@
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A456" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B456" t="s">
         <v>439</v>
@@ -21918,7 +21918,7 @@
         <v>443</v>
       </c>
       <c r="E456" t="s">
-        <v>208</v>
+        <v>339</v>
       </c>
       <c r="F456" t="s">
         <v>454</v>
@@ -21926,7 +21926,7 @@
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A457" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B457" t="s">
         <v>439</v>
@@ -21938,7 +21938,7 @@
         <v>447</v>
       </c>
       <c r="E457" t="s">
-        <v>208</v>
+        <v>339</v>
       </c>
       <c r="F457" t="s">
         <v>454</v>
@@ -21958,7 +21958,7 @@
         <v>441</v>
       </c>
       <c r="E458" t="s">
-        <v>340</v>
+        <v>208</v>
       </c>
       <c r="F458" t="s">
         <v>454</v>
@@ -21978,7 +21978,7 @@
         <v>451</v>
       </c>
       <c r="E459" t="s">
-        <v>340</v>
+        <v>208</v>
       </c>
       <c r="F459" t="s">
         <v>454</v>
@@ -21998,7 +21998,7 @@
         <v>449</v>
       </c>
       <c r="E460" t="s">
-        <v>340</v>
+        <v>208</v>
       </c>
       <c r="F460" t="s">
         <v>454</v>
@@ -22018,7 +22018,7 @@
         <v>445</v>
       </c>
       <c r="E461" t="s">
-        <v>340</v>
+        <v>208</v>
       </c>
       <c r="F461" t="s">
         <v>454</v>
@@ -22038,7 +22038,7 @@
         <v>443</v>
       </c>
       <c r="E462" t="s">
-        <v>340</v>
+        <v>208</v>
       </c>
       <c r="F462" t="s">
         <v>454</v>
@@ -22058,7 +22058,7 @@
         <v>447</v>
       </c>
       <c r="E463" t="s">
-        <v>340</v>
+        <v>208</v>
       </c>
       <c r="F463" t="s">
         <v>454</v>
@@ -22066,7 +22066,7 @@
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A464" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B464" t="s">
         <v>439</v>
@@ -22078,7 +22078,7 @@
         <v>441</v>
       </c>
       <c r="E464" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F464" t="s">
         <v>454</v>
@@ -22086,7 +22086,7 @@
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A465" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B465" t="s">
         <v>439</v>
@@ -22098,7 +22098,7 @@
         <v>451</v>
       </c>
       <c r="E465" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F465" t="s">
         <v>454</v>
@@ -22106,7 +22106,7 @@
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A466" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B466" t="s">
         <v>439</v>
@@ -22118,7 +22118,7 @@
         <v>449</v>
       </c>
       <c r="E466" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F466" t="s">
         <v>454</v>
@@ -22126,7 +22126,7 @@
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A467" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B467" t="s">
         <v>439</v>
@@ -22138,7 +22138,7 @@
         <v>445</v>
       </c>
       <c r="E467" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F467" t="s">
         <v>454</v>
@@ -22146,7 +22146,7 @@
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A468" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B468" t="s">
         <v>439</v>
@@ -22158,7 +22158,7 @@
         <v>443</v>
       </c>
       <c r="E468" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F468" t="s">
         <v>454</v>
@@ -22166,7 +22166,7 @@
     </row>
     <row r="469" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A469" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B469" t="s">
         <v>439</v>
@@ -22178,7 +22178,7 @@
         <v>447</v>
       </c>
       <c r="E469" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F469" t="s">
         <v>454</v>
@@ -22198,7 +22198,7 @@
         <v>441</v>
       </c>
       <c r="E470" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="F470" t="s">
         <v>454</v>
@@ -22218,7 +22218,7 @@
         <v>451</v>
       </c>
       <c r="E471" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="F471" t="s">
         <v>454</v>
@@ -22238,7 +22238,7 @@
         <v>449</v>
       </c>
       <c r="E472" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="F472" t="s">
         <v>454</v>
@@ -22258,7 +22258,7 @@
         <v>445</v>
       </c>
       <c r="E473" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="F473" t="s">
         <v>454</v>
@@ -22278,7 +22278,7 @@
         <v>443</v>
       </c>
       <c r="E474" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="F474" t="s">
         <v>454</v>
@@ -22298,7 +22298,7 @@
         <v>447</v>
       </c>
       <c r="E475" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="F475" t="s">
         <v>454</v>
@@ -22306,7 +22306,7 @@
     </row>
     <row r="476" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A476" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B476" t="s">
         <v>439</v>
@@ -22318,7 +22318,7 @@
         <v>441</v>
       </c>
       <c r="E476" t="s">
-        <v>377</v>
+        <v>203</v>
       </c>
       <c r="F476" t="s">
         <v>454</v>
@@ -22326,7 +22326,7 @@
     </row>
     <row r="477" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A477" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B477" t="s">
         <v>439</v>
@@ -22338,7 +22338,7 @@
         <v>451</v>
       </c>
       <c r="E477" t="s">
-        <v>377</v>
+        <v>203</v>
       </c>
       <c r="F477" t="s">
         <v>454</v>
@@ -22346,7 +22346,7 @@
     </row>
     <row r="478" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A478" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B478" t="s">
         <v>439</v>
@@ -22358,7 +22358,7 @@
         <v>449</v>
       </c>
       <c r="E478" t="s">
-        <v>377</v>
+        <v>203</v>
       </c>
       <c r="F478" t="s">
         <v>454</v>
@@ -22366,7 +22366,7 @@
     </row>
     <row r="479" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A479" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B479" t="s">
         <v>439</v>
@@ -22378,7 +22378,7 @@
         <v>445</v>
       </c>
       <c r="E479" t="s">
-        <v>377</v>
+        <v>203</v>
       </c>
       <c r="F479" t="s">
         <v>454</v>
@@ -22386,7 +22386,7 @@
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A480" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B480" t="s">
         <v>439</v>
@@ -22398,7 +22398,7 @@
         <v>443</v>
       </c>
       <c r="E480" t="s">
-        <v>377</v>
+        <v>203</v>
       </c>
       <c r="F480" t="s">
         <v>454</v>
@@ -22406,7 +22406,7 @@
     </row>
     <row r="481" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A481" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B481" t="s">
         <v>439</v>
@@ -22418,7 +22418,7 @@
         <v>447</v>
       </c>
       <c r="E481" t="s">
-        <v>377</v>
+        <v>203</v>
       </c>
       <c r="F481" t="s">
         <v>454</v>
@@ -22426,7 +22426,7 @@
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A482" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B482" t="s">
         <v>439</v>
@@ -22438,7 +22438,7 @@
         <v>441</v>
       </c>
       <c r="E482" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F482" t="s">
         <v>454</v>
@@ -22446,7 +22446,7 @@
     </row>
     <row r="483" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A483" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B483" t="s">
         <v>439</v>
@@ -22458,7 +22458,7 @@
         <v>451</v>
       </c>
       <c r="E483" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F483" t="s">
         <v>454</v>
@@ -22466,7 +22466,7 @@
     </row>
     <row r="484" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A484" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B484" t="s">
         <v>439</v>
@@ -22478,7 +22478,7 @@
         <v>449</v>
       </c>
       <c r="E484" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F484" t="s">
         <v>454</v>
@@ -22486,7 +22486,7 @@
     </row>
     <row r="485" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A485" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B485" t="s">
         <v>439</v>
@@ -22498,7 +22498,7 @@
         <v>445</v>
       </c>
       <c r="E485" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F485" t="s">
         <v>454</v>
@@ -22506,7 +22506,7 @@
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A486" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B486" t="s">
         <v>439</v>
@@ -22518,7 +22518,7 @@
         <v>443</v>
       </c>
       <c r="E486" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F486" t="s">
         <v>454</v>
@@ -22526,7 +22526,7 @@
     </row>
     <row r="487" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A487" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B487" t="s">
         <v>439</v>
@@ -22538,7 +22538,7 @@
         <v>447</v>
       </c>
       <c r="E487" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F487" t="s">
         <v>454</v>
@@ -22546,7 +22546,7 @@
     </row>
     <row r="488" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A488" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B488" t="s">
         <v>439</v>
@@ -22558,7 +22558,7 @@
         <v>441</v>
       </c>
       <c r="E488" t="s">
-        <v>189</v>
+        <v>366</v>
       </c>
       <c r="F488" t="s">
         <v>454</v>
@@ -22566,7 +22566,7 @@
     </row>
     <row r="489" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A489" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B489" t="s">
         <v>439</v>
@@ -22578,7 +22578,7 @@
         <v>451</v>
       </c>
       <c r="E489" t="s">
-        <v>189</v>
+        <v>366</v>
       </c>
       <c r="F489" t="s">
         <v>454</v>
@@ -22586,7 +22586,7 @@
     </row>
     <row r="490" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A490" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B490" t="s">
         <v>439</v>
@@ -22598,7 +22598,7 @@
         <v>449</v>
       </c>
       <c r="E490" t="s">
-        <v>189</v>
+        <v>366</v>
       </c>
       <c r="F490" t="s">
         <v>454</v>
@@ -22606,7 +22606,7 @@
     </row>
     <row r="491" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A491" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B491" t="s">
         <v>439</v>
@@ -22618,7 +22618,7 @@
         <v>445</v>
       </c>
       <c r="E491" t="s">
-        <v>189</v>
+        <v>366</v>
       </c>
       <c r="F491" t="s">
         <v>454</v>
@@ -22626,7 +22626,7 @@
     </row>
     <row r="492" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A492" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B492" t="s">
         <v>439</v>
@@ -22638,7 +22638,7 @@
         <v>443</v>
       </c>
       <c r="E492" t="s">
-        <v>189</v>
+        <v>366</v>
       </c>
       <c r="F492" t="s">
         <v>454</v>
@@ -22646,7 +22646,7 @@
     </row>
     <row r="493" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A493" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B493" t="s">
         <v>439</v>
@@ -22658,7 +22658,7 @@
         <v>447</v>
       </c>
       <c r="E493" t="s">
-        <v>189</v>
+        <v>366</v>
       </c>
       <c r="F493" t="s">
         <v>454</v>
@@ -22678,7 +22678,7 @@
         <v>441</v>
       </c>
       <c r="E494" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="F494" t="s">
         <v>454</v>
@@ -22698,7 +22698,7 @@
         <v>451</v>
       </c>
       <c r="E495" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="F495" t="s">
         <v>454</v>
@@ -22718,7 +22718,7 @@
         <v>449</v>
       </c>
       <c r="E496" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="F496" t="s">
         <v>454</v>
@@ -22738,7 +22738,7 @@
         <v>445</v>
       </c>
       <c r="E497" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="F497" t="s">
         <v>454</v>
@@ -22758,7 +22758,7 @@
         <v>443</v>
       </c>
       <c r="E498" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="F498" t="s">
         <v>454</v>
@@ -22778,7 +22778,7 @@
         <v>447</v>
       </c>
       <c r="E499" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="F499" t="s">
         <v>454</v>
@@ -22786,7 +22786,7 @@
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A500" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B500" t="s">
         <v>439</v>
@@ -22798,7 +22798,7 @@
         <v>441</v>
       </c>
       <c r="E500" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="F500" t="s">
         <v>454</v>
@@ -22806,7 +22806,7 @@
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A501" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B501" t="s">
         <v>439</v>
@@ -22818,7 +22818,7 @@
         <v>451</v>
       </c>
       <c r="E501" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="F501" t="s">
         <v>454</v>
@@ -22826,7 +22826,7 @@
     </row>
     <row r="502" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A502" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B502" t="s">
         <v>439</v>
@@ -22838,7 +22838,7 @@
         <v>449</v>
       </c>
       <c r="E502" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="F502" t="s">
         <v>454</v>
@@ -22846,7 +22846,7 @@
     </row>
     <row r="503" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A503" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B503" t="s">
         <v>439</v>
@@ -22858,7 +22858,7 @@
         <v>445</v>
       </c>
       <c r="E503" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="F503" t="s">
         <v>454</v>
@@ -22866,7 +22866,7 @@
     </row>
     <row r="504" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A504" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B504" t="s">
         <v>439</v>
@@ -22878,7 +22878,7 @@
         <v>443</v>
       </c>
       <c r="E504" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="F504" t="s">
         <v>454</v>
@@ -22886,7 +22886,7 @@
     </row>
     <row r="505" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A505" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B505" t="s">
         <v>439</v>
@@ -22898,7 +22898,7 @@
         <v>447</v>
       </c>
       <c r="E505" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="F505" t="s">
         <v>454</v>
@@ -22918,7 +22918,7 @@
         <v>441</v>
       </c>
       <c r="E506" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F506" t="s">
         <v>454</v>
@@ -22938,7 +22938,7 @@
         <v>451</v>
       </c>
       <c r="E507" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F507" t="s">
         <v>454</v>
@@ -22958,7 +22958,7 @@
         <v>449</v>
       </c>
       <c r="E508" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F508" t="s">
         <v>454</v>
@@ -22978,7 +22978,7 @@
         <v>445</v>
       </c>
       <c r="E509" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F509" t="s">
         <v>454</v>
@@ -22998,7 +22998,7 @@
         <v>443</v>
       </c>
       <c r="E510" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F510" t="s">
         <v>454</v>
@@ -23018,7 +23018,7 @@
         <v>447</v>
       </c>
       <c r="E511" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F511" t="s">
         <v>454</v>
@@ -23038,7 +23038,7 @@
         <v>441</v>
       </c>
       <c r="E512" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="F512" t="s">
         <v>454</v>
@@ -23058,7 +23058,7 @@
         <v>451</v>
       </c>
       <c r="E513" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="F513" t="s">
         <v>454</v>
@@ -23078,7 +23078,7 @@
         <v>449</v>
       </c>
       <c r="E514" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="F514" t="s">
         <v>454</v>
@@ -23098,7 +23098,7 @@
         <v>445</v>
       </c>
       <c r="E515" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="F515" t="s">
         <v>454</v>
@@ -23118,7 +23118,7 @@
         <v>443</v>
       </c>
       <c r="E516" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="F516" t="s">
         <v>454</v>
@@ -23138,7 +23138,7 @@
         <v>447</v>
       </c>
       <c r="E517" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="F517" t="s">
         <v>454</v>
@@ -23158,7 +23158,7 @@
         <v>441</v>
       </c>
       <c r="E518" t="s">
-        <v>319</v>
+        <v>34</v>
       </c>
       <c r="F518" t="s">
         <v>454</v>
@@ -23178,7 +23178,7 @@
         <v>451</v>
       </c>
       <c r="E519" t="s">
-        <v>319</v>
+        <v>34</v>
       </c>
       <c r="F519" t="s">
         <v>454</v>
@@ -23198,7 +23198,7 @@
         <v>449</v>
       </c>
       <c r="E520" t="s">
-        <v>319</v>
+        <v>34</v>
       </c>
       <c r="F520" t="s">
         <v>454</v>
@@ -23218,7 +23218,7 @@
         <v>445</v>
       </c>
       <c r="E521" t="s">
-        <v>319</v>
+        <v>34</v>
       </c>
       <c r="F521" t="s">
         <v>454</v>
@@ -23238,7 +23238,7 @@
         <v>443</v>
       </c>
       <c r="E522" t="s">
-        <v>319</v>
+        <v>34</v>
       </c>
       <c r="F522" t="s">
         <v>454</v>
@@ -23258,7 +23258,7 @@
         <v>447</v>
       </c>
       <c r="E523" t="s">
-        <v>319</v>
+        <v>34</v>
       </c>
       <c r="F523" t="s">
         <v>454</v>
@@ -23278,7 +23278,7 @@
         <v>441</v>
       </c>
       <c r="E524" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F524" t="s">
         <v>454</v>
@@ -23298,7 +23298,7 @@
         <v>451</v>
       </c>
       <c r="E525" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F525" t="s">
         <v>454</v>
@@ -23318,7 +23318,7 @@
         <v>449</v>
       </c>
       <c r="E526" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F526" t="s">
         <v>454</v>
@@ -23338,7 +23338,7 @@
         <v>445</v>
       </c>
       <c r="E527" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F527" t="s">
         <v>454</v>
@@ -23358,7 +23358,7 @@
         <v>443</v>
       </c>
       <c r="E528" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F528" t="s">
         <v>454</v>
@@ -23378,7 +23378,7 @@
         <v>447</v>
       </c>
       <c r="E529" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F529" t="s">
         <v>454</v>
@@ -23386,7 +23386,7 @@
     </row>
     <row r="530" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A530" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B530" t="s">
         <v>439</v>
@@ -23398,7 +23398,7 @@
         <v>441</v>
       </c>
       <c r="E530" t="s">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="F530" t="s">
         <v>454</v>
@@ -23406,7 +23406,7 @@
     </row>
     <row r="531" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A531" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B531" t="s">
         <v>439</v>
@@ -23418,7 +23418,7 @@
         <v>451</v>
       </c>
       <c r="E531" t="s">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="F531" t="s">
         <v>454</v>
@@ -23426,7 +23426,7 @@
     </row>
     <row r="532" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A532" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B532" t="s">
         <v>439</v>
@@ -23438,7 +23438,7 @@
         <v>449</v>
       </c>
       <c r="E532" t="s">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="F532" t="s">
         <v>454</v>
@@ -23446,7 +23446,7 @@
     </row>
     <row r="533" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A533" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B533" t="s">
         <v>439</v>
@@ -23458,7 +23458,7 @@
         <v>445</v>
       </c>
       <c r="E533" t="s">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="F533" t="s">
         <v>454</v>
@@ -23466,7 +23466,7 @@
     </row>
     <row r="534" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A534" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B534" t="s">
         <v>439</v>
@@ -23478,7 +23478,7 @@
         <v>443</v>
       </c>
       <c r="E534" t="s">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="F534" t="s">
         <v>454</v>
@@ -23486,7 +23486,7 @@
     </row>
     <row r="535" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A535" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B535" t="s">
         <v>439</v>
@@ -23498,7 +23498,7 @@
         <v>447</v>
       </c>
       <c r="E535" t="s">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="F535" t="s">
         <v>454</v>
@@ -23518,7 +23518,7 @@
         <v>441</v>
       </c>
       <c r="E536" t="s">
-        <v>342</v>
+        <v>204</v>
       </c>
       <c r="F536" t="s">
         <v>454</v>
@@ -23538,7 +23538,7 @@
         <v>451</v>
       </c>
       <c r="E537" t="s">
-        <v>342</v>
+        <v>204</v>
       </c>
       <c r="F537" t="s">
         <v>454</v>
@@ -23558,7 +23558,7 @@
         <v>449</v>
       </c>
       <c r="E538" t="s">
-        <v>342</v>
+        <v>204</v>
       </c>
       <c r="F538" t="s">
         <v>454</v>
@@ -23578,7 +23578,7 @@
         <v>445</v>
       </c>
       <c r="E539" t="s">
-        <v>342</v>
+        <v>204</v>
       </c>
       <c r="F539" t="s">
         <v>454</v>
@@ -23598,7 +23598,7 @@
         <v>443</v>
       </c>
       <c r="E540" t="s">
-        <v>342</v>
+        <v>204</v>
       </c>
       <c r="F540" t="s">
         <v>454</v>
@@ -23618,7 +23618,7 @@
         <v>447</v>
       </c>
       <c r="E541" t="s">
-        <v>342</v>
+        <v>204</v>
       </c>
       <c r="F541" t="s">
         <v>454</v>
@@ -23626,7 +23626,7 @@
     </row>
     <row r="542" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A542" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B542" t="s">
         <v>439</v>
@@ -23638,7 +23638,7 @@
         <v>441</v>
       </c>
       <c r="E542" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="F542" t="s">
         <v>454</v>
@@ -23646,7 +23646,7 @@
     </row>
     <row r="543" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A543" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B543" t="s">
         <v>439</v>
@@ -23658,7 +23658,7 @@
         <v>451</v>
       </c>
       <c r="E543" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="F543" t="s">
         <v>454</v>
@@ -23666,7 +23666,7 @@
     </row>
     <row r="544" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A544" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B544" t="s">
         <v>439</v>
@@ -23678,7 +23678,7 @@
         <v>449</v>
       </c>
       <c r="E544" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="F544" t="s">
         <v>454</v>
@@ -23686,7 +23686,7 @@
     </row>
     <row r="545" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A545" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B545" t="s">
         <v>439</v>
@@ -23698,7 +23698,7 @@
         <v>445</v>
       </c>
       <c r="E545" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="F545" t="s">
         <v>454</v>
@@ -23706,7 +23706,7 @@
     </row>
     <row r="546" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A546" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B546" t="s">
         <v>439</v>
@@ -23718,7 +23718,7 @@
         <v>443</v>
       </c>
       <c r="E546" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="F546" t="s">
         <v>454</v>
@@ -23726,7 +23726,7 @@
     </row>
     <row r="547" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A547" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B547" t="s">
         <v>439</v>
@@ -23738,7 +23738,7 @@
         <v>447</v>
       </c>
       <c r="E547" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="F547" t="s">
         <v>454</v>
@@ -23758,7 +23758,7 @@
         <v>441</v>
       </c>
       <c r="E548" t="s">
-        <v>341</v>
+        <v>205</v>
       </c>
       <c r="F548" t="s">
         <v>454</v>
@@ -23778,7 +23778,7 @@
         <v>451</v>
       </c>
       <c r="E549" t="s">
-        <v>341</v>
+        <v>205</v>
       </c>
       <c r="F549" t="s">
         <v>454</v>
@@ -23798,7 +23798,7 @@
         <v>449</v>
       </c>
       <c r="E550" t="s">
-        <v>341</v>
+        <v>205</v>
       </c>
       <c r="F550" t="s">
         <v>454</v>
@@ -23818,7 +23818,7 @@
         <v>445</v>
       </c>
       <c r="E551" t="s">
-        <v>341</v>
+        <v>205</v>
       </c>
       <c r="F551" t="s">
         <v>454</v>
@@ -23838,7 +23838,7 @@
         <v>443</v>
       </c>
       <c r="E552" t="s">
-        <v>341</v>
+        <v>205</v>
       </c>
       <c r="F552" t="s">
         <v>454</v>
@@ -23858,7 +23858,7 @@
         <v>447</v>
       </c>
       <c r="E553" t="s">
-        <v>341</v>
+        <v>205</v>
       </c>
       <c r="F553" t="s">
         <v>454</v>
@@ -23866,7 +23866,7 @@
     </row>
     <row r="554" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A554" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B554" t="s">
         <v>439</v>
@@ -23878,7 +23878,7 @@
         <v>441</v>
       </c>
       <c r="E554" t="s">
-        <v>88</v>
+        <v>341</v>
       </c>
       <c r="F554" t="s">
         <v>454</v>
@@ -23886,7 +23886,7 @@
     </row>
     <row r="555" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A555" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B555" t="s">
         <v>439</v>
@@ -23898,7 +23898,7 @@
         <v>451</v>
       </c>
       <c r="E555" t="s">
-        <v>88</v>
+        <v>341</v>
       </c>
       <c r="F555" t="s">
         <v>454</v>
@@ -23906,7 +23906,7 @@
     </row>
     <row r="556" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A556" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B556" t="s">
         <v>439</v>
@@ -23918,7 +23918,7 @@
         <v>449</v>
       </c>
       <c r="E556" t="s">
-        <v>88</v>
+        <v>341</v>
       </c>
       <c r="F556" t="s">
         <v>454</v>
@@ -23926,7 +23926,7 @@
     </row>
     <row r="557" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A557" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B557" t="s">
         <v>439</v>
@@ -23938,7 +23938,7 @@
         <v>445</v>
       </c>
       <c r="E557" t="s">
-        <v>88</v>
+        <v>341</v>
       </c>
       <c r="F557" t="s">
         <v>454</v>
@@ -23946,7 +23946,7 @@
     </row>
     <row r="558" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A558" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B558" t="s">
         <v>439</v>
@@ -23958,7 +23958,7 @@
         <v>443</v>
       </c>
       <c r="E558" t="s">
-        <v>88</v>
+        <v>341</v>
       </c>
       <c r="F558" t="s">
         <v>454</v>
@@ -23966,7 +23966,7 @@
     </row>
     <row r="559" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A559" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B559" t="s">
         <v>439</v>
@@ -23978,7 +23978,7 @@
         <v>447</v>
       </c>
       <c r="E559" t="s">
-        <v>88</v>
+        <v>341</v>
       </c>
       <c r="F559" t="s">
         <v>454</v>
@@ -23998,7 +23998,7 @@
         <v>441</v>
       </c>
       <c r="E560" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
       <c r="F560" t="s">
         <v>454</v>
@@ -24018,7 +24018,7 @@
         <v>451</v>
       </c>
       <c r="E561" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
       <c r="F561" t="s">
         <v>454</v>
@@ -24038,7 +24038,7 @@
         <v>449</v>
       </c>
       <c r="E562" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
       <c r="F562" t="s">
         <v>454</v>
@@ -24058,7 +24058,7 @@
         <v>445</v>
       </c>
       <c r="E563" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
       <c r="F563" t="s">
         <v>454</v>
@@ -24078,7 +24078,7 @@
         <v>443</v>
       </c>
       <c r="E564" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
       <c r="F564" t="s">
         <v>454</v>
@@ -24098,7 +24098,7 @@
         <v>447</v>
       </c>
       <c r="E565" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
       <c r="F565" t="s">
         <v>454</v>
@@ -24118,7 +24118,7 @@
         <v>441</v>
       </c>
       <c r="E566" t="s">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="F566" t="s">
         <v>454</v>
@@ -24138,7 +24138,7 @@
         <v>451</v>
       </c>
       <c r="E567" t="s">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="F567" t="s">
         <v>454</v>
@@ -24158,7 +24158,7 @@
         <v>449</v>
       </c>
       <c r="E568" t="s">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="F568" t="s">
         <v>454</v>
@@ -24178,7 +24178,7 @@
         <v>445</v>
       </c>
       <c r="E569" t="s">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="F569" t="s">
         <v>454</v>
@@ -24198,7 +24198,7 @@
         <v>443</v>
       </c>
       <c r="E570" t="s">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="F570" t="s">
         <v>454</v>
@@ -24218,7 +24218,7 @@
         <v>447</v>
       </c>
       <c r="E571" t="s">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="F571" t="s">
         <v>454</v>
@@ -24238,7 +24238,7 @@
         <v>441</v>
       </c>
       <c r="E572" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F572" t="s">
         <v>454</v>
@@ -24258,7 +24258,7 @@
         <v>451</v>
       </c>
       <c r="E573" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F573" t="s">
         <v>454</v>
@@ -24278,7 +24278,7 @@
         <v>449</v>
       </c>
       <c r="E574" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F574" t="s">
         <v>454</v>
@@ -24298,7 +24298,7 @@
         <v>445</v>
       </c>
       <c r="E575" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F575" t="s">
         <v>454</v>
@@ -24318,7 +24318,7 @@
         <v>443</v>
       </c>
       <c r="E576" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F576" t="s">
         <v>454</v>
@@ -24338,7 +24338,7 @@
         <v>447</v>
       </c>
       <c r="E577" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F577" t="s">
         <v>454</v>
@@ -24358,7 +24358,7 @@
         <v>441</v>
       </c>
       <c r="E578" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F578" t="s">
         <v>454</v>
@@ -24378,7 +24378,7 @@
         <v>451</v>
       </c>
       <c r="E579" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F579" t="s">
         <v>454</v>
@@ -24398,7 +24398,7 @@
         <v>449</v>
       </c>
       <c r="E580" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F580" t="s">
         <v>454</v>
@@ -24418,7 +24418,7 @@
         <v>445</v>
       </c>
       <c r="E581" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F581" t="s">
         <v>454</v>
@@ -24438,7 +24438,7 @@
         <v>443</v>
       </c>
       <c r="E582" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F582" t="s">
         <v>454</v>
@@ -24458,7 +24458,7 @@
         <v>447</v>
       </c>
       <c r="E583" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F583" t="s">
         <v>454</v>
@@ -24466,7 +24466,7 @@
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A584" t="s">
-        <v>442</v>
+        <v>15</v>
       </c>
       <c r="B584" t="s">
         <v>439</v>
@@ -24478,7 +24478,7 @@
         <v>441</v>
       </c>
       <c r="E584" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="F584" t="s">
         <v>454</v>
@@ -24486,7 +24486,7 @@
     </row>
     <row r="585" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A585" t="s">
-        <v>442</v>
+        <v>15</v>
       </c>
       <c r="B585" t="s">
         <v>439</v>
@@ -24498,7 +24498,7 @@
         <v>451</v>
       </c>
       <c r="E585" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="F585" t="s">
         <v>454</v>
@@ -24506,7 +24506,7 @@
     </row>
     <row r="586" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A586" t="s">
-        <v>442</v>
+        <v>15</v>
       </c>
       <c r="B586" t="s">
         <v>439</v>
@@ -24518,7 +24518,7 @@
         <v>449</v>
       </c>
       <c r="E586" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="F586" t="s">
         <v>454</v>
@@ -24526,7 +24526,7 @@
     </row>
     <row r="587" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A587" t="s">
-        <v>442</v>
+        <v>15</v>
       </c>
       <c r="B587" t="s">
         <v>439</v>
@@ -24538,7 +24538,7 @@
         <v>445</v>
       </c>
       <c r="E587" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="F587" t="s">
         <v>454</v>
@@ -24546,7 +24546,7 @@
     </row>
     <row r="588" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A588" t="s">
-        <v>442</v>
+        <v>15</v>
       </c>
       <c r="B588" t="s">
         <v>439</v>
@@ -24558,7 +24558,7 @@
         <v>443</v>
       </c>
       <c r="E588" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="F588" t="s">
         <v>454</v>
@@ -24566,7 +24566,7 @@
     </row>
     <row r="589" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A589" t="s">
-        <v>442</v>
+        <v>15</v>
       </c>
       <c r="B589" t="s">
         <v>439</v>
@@ -24578,7 +24578,7 @@
         <v>447</v>
       </c>
       <c r="E589" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="F589" t="s">
         <v>454</v>
@@ -27225,7 +27225,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F721"/>
+  <autoFilter ref="A1:F721">
+    <sortState ref="A2:F721">
+      <sortCondition ref="A1:A721"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>